<commit_message>
Add sum in timetable
</commit_message>
<xml_diff>
--- a/doc/Zeitabrechnung.xlsx
+++ b/doc/Zeitabrechnung.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Robert</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>Kholoud</t>
+  </si>
+  <si>
+    <t>SUM:</t>
   </si>
 </sst>
 </file>
@@ -57,7 +60,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -70,6 +73,7 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -337,27 +341,27 @@
       <c r="A9" s="2">
         <v>45240.0</v>
       </c>
-      <c r="C9" s="3">
-        <v>0.041666666666666664</v>
+      <c r="C9" s="1">
+        <v>1.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
         <v>45241.0</v>
       </c>
-      <c r="B10" s="3">
-        <v>0.125</v>
+      <c r="B10" s="1">
+        <v>3.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
         <v>45242.0</v>
       </c>
-      <c r="B11" s="3">
-        <v>0.041666666666666664</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0.041666666666666664</v>
+      <c r="B11" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1.0</v>
       </c>
     </row>
     <row r="12">
@@ -464,8 +468,8 @@
       <c r="A32" s="2">
         <v>45263.0</v>
       </c>
-      <c r="B32" s="3">
-        <v>0.041666666666666664</v>
+      <c r="B32" s="1">
+        <v>1.0</v>
       </c>
     </row>
     <row r="33">
@@ -477,11 +481,11 @@
       <c r="A34" s="2">
         <v>45265.0</v>
       </c>
-      <c r="B34" s="3">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C34" s="3">
-        <v>0.125</v>
+      <c r="B34" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C34" s="1">
+        <v>3.0</v>
       </c>
       <c r="D34" s="3"/>
     </row>
@@ -495,60 +499,535 @@
       <c r="A36" s="2">
         <v>45267.0</v>
       </c>
-      <c r="C36" s="3">
-        <v>0.20833333333333334</v>
-      </c>
-      <c r="D36" s="3">
-        <v>0.2916666666666667</v>
+      <c r="C36" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>7.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
         <v>45268.0</v>
       </c>
-      <c r="B37" s="3">
-        <v>0.125</v>
-      </c>
-      <c r="C37" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="D37" s="3">
-        <v>0.375</v>
+      <c r="B37" s="1">
+        <v>3.0</v>
+      </c>
+      <c r="C37" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>9.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
         <v>45269.0</v>
       </c>
-      <c r="B38" s="3">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="C38" s="3">
-        <v>0.20833333333333334</v>
+      <c r="B38" s="1">
+        <v>4.0</v>
+      </c>
+      <c r="C38" s="1">
+        <v>5.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
         <v>45270.0</v>
       </c>
-      <c r="B39" s="3">
-        <v>0.25</v>
-      </c>
-      <c r="C39" s="3">
-        <v>0.25</v>
+      <c r="B39" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="C39" s="1">
+        <v>6.0</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="2"/>
+      <c r="A40" s="2">
+        <v>45271.0</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="2"/>
+      <c r="A41" s="2">
+        <v>45272.0</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="2"/>
+      <c r="A42" s="2">
+        <v>45273.0</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="2"/>
+      <c r="A43" s="2">
+        <v>45274.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2">
+        <v>45275.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2">
+        <v>45276.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2">
+        <v>45277.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2">
+        <v>45278.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2">
+        <v>45279.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2">
+        <v>45280.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2">
+        <v>45281.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2">
+        <v>45282.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2">
+        <v>45283.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2">
+        <v>45284.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2">
+        <v>45285.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2">
+        <v>45286.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2">
+        <v>45287.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2">
+        <v>45288.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2">
+        <v>45289.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2">
+        <v>45290.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2">
+        <v>45291.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2">
+        <v>45292.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2">
+        <v>45293.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2">
+        <v>45294.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2">
+        <v>45295.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2">
+        <v>45296.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2">
+        <v>45297.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2">
+        <v>45298.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2">
+        <v>45299.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2">
+        <v>45300.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2">
+        <v>45301.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2">
+        <v>45302.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2">
+        <v>45303.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2">
+        <v>45304.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2">
+        <v>45305.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2">
+        <v>45306.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2">
+        <v>45307.0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2">
+        <v>45308.0</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2">
+        <v>45309.0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2">
+        <v>45310.0</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2">
+        <v>45311.0</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2">
+        <v>45312.0</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2">
+        <v>45313.0</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2">
+        <v>45314.0</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2">
+        <v>45315.0</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2">
+        <v>45316.0</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2">
+        <v>45317.0</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2">
+        <v>45318.0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2">
+        <v>45319.0</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2">
+        <v>45320.0</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2">
+        <v>45321.0</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2">
+        <v>45322.0</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2">
+        <v>45323.0</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2">
+        <v>45324.0</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2">
+        <v>45325.0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2">
+        <v>45326.0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2">
+        <v>45327.0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2">
+        <v>45328.0</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2">
+        <v>45329.0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2">
+        <v>45330.0</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2">
+        <v>45331.0</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2">
+        <v>45332.0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2">
+        <v>45333.0</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2">
+        <v>45334.0</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2">
+        <v>45335.0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2">
+        <v>45336.0</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2">
+        <v>45337.0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2">
+        <v>45338.0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2">
+        <v>45339.0</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2">
+        <v>45340.0</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2">
+        <v>45341.0</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2">
+        <v>45342.0</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2">
+        <v>45343.0</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2">
+        <v>45344.0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2">
+        <v>45345.0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2">
+        <v>45346.0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2">
+        <v>45347.0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2">
+        <v>45348.0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2">
+        <v>45349.0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2">
+        <v>45350.0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2">
+        <v>45351.0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2">
+        <v>45352.0</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2">
+        <v>45353.0</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2">
+        <v>45354.0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2">
+        <v>45355.0</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2">
+        <v>45356.0</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2">
+        <v>45357.0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2">
+        <v>45358.0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2">
+        <v>45359.0</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2">
+        <v>45360.0</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2">
+        <v>45361.0</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2">
+        <v>45362.0</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2">
+        <v>45363.0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="2">
+        <v>45364.0</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B134" s="4">
+        <f t="shared" ref="B134:D134" si="1">SUM(B2:B133)</f>
+        <v>22</v>
+      </c>
+      <c r="C134" s="4">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="D134" s="4">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>